<commit_message>
Updated CCS files with new model version
</commit_message>
<xml_diff>
--- a/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
+++ b/InputData/ccs/CCP/CO2 Capture Potentials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\ccs\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C486A-5B60-4A9B-B6D8-7B42A078F02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6405BF9F-1D3A-4C50-AE6F-24D97B944D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="25020" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="510" windowWidth="24540" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Source:</t>
   </si>
@@ -229,6 +229,12 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>energy related emissions</t>
+  </si>
+  <si>
+    <t>process emissions</t>
   </si>
 </sst>
 </file>
@@ -942,81 +948,113 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
     </row>

</xml_diff>